<commit_message>
issue #173 - fix CellRange reset change matrix
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue173Test.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue173Test.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C85714-EFF9-45CD-A862-5FD72B869570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="337" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24195" windowHeight="13695" tabRatio="337"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -33,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Marcus Warm</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="A9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="C10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="A15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\/mm"/>
     <numFmt numFmtId="165" formatCode="#,##0;[Red]\-#,##0;0"/>
@@ -270,7 +264,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +293,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -365,25 +383,14 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -400,19 +407,35 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Pivot Tabelle Ecke" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Pivot Tabelle Ergebnis" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Pivot Tabelle Feld" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Pivot Tabelle Kategorie" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Pivot Tabelle Titel" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Pivot Tabelle Wert" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Pivot Tabelle Ecke" xfId="1"/>
+    <cellStyle name="Pivot Tabelle Ergebnis" xfId="2"/>
+    <cellStyle name="Pivot Tabelle Feld" xfId="3"/>
+    <cellStyle name="Pivot Tabelle Kategorie" xfId="4"/>
+    <cellStyle name="Pivot Tabelle Titel" xfId="5"/>
+    <cellStyle name="Pivot Tabelle Wert" xfId="6"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -835,90 +858,95 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:27" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="C3" s="14"/>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="C3" s="9"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="16"/>
-      <c r="E4" s="1"/>
-      <c r="I4" s="4"/>
-      <c r="AA4" s="4"/>
-    </row>
-    <row r="5" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="15"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="16"/>
+      <c r="I4" s="2"/>
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19">
         <f>SUM(C9)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B10" s="17">
+      <c r="C9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:27" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B10" s="11">
         <f>SUM(B9)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:27" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>